<commit_message>
correcciones main y modulo mux
</commit_message>
<xml_diff>
--- a/Dedicación horaria semanal.xlsx
+++ b/Dedicación horaria semanal.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t xml:space="preserve">Henry</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">no se registro dedicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hito</t>
   </si>
 </sst>
 </file>
@@ -179,7 +182,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,7 +192,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFB7E1CD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -208,6 +211,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF9900"/>
         <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF66"/>
+        <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -258,7 +267,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -303,7 +312,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -312,6 +329,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -324,21 +345,12 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00FF66"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -369,7 +381,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFB7E1CD"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -401,15 +413,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y32"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+      <selection pane="topLeft" activeCell="I34" activeCellId="0" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="13.6326530612245"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1637,28 +1649,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="5" t="n">
+      <c r="B26" s="11"/>
+      <c r="C26" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="H26" s="6" t="n">
-        <v>0</v>
-      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="11"/>
       <c r="I26" s="7" t="n">
         <f aca="false">SUM(B26:H26)</f>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1683,7 +1689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>36</v>
       </c>
@@ -1798,23 +1804,29 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I30" s="11" t="n">
+      <c r="I30" s="13" t="n">
         <f aca="false">SUM(I3:I29)</f>
-        <v>264.96</v>
-      </c>
-      <c r="Q30" s="11" t="n">
+        <v>254.96</v>
+      </c>
+      <c r="Q30" s="13" t="n">
         <f aca="false">SUM(Q3:Q29)</f>
         <v>116.4</v>
       </c>
-      <c r="Y30" s="11" t="n">
+      <c r="Y30" s="13" t="n">
         <f aca="false">SUM(Y3:Y29)</f>
         <v>110.05</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="12"/>
-      <c r="D32" s="13" t="s">
+      <c r="C32" s="14"/>
+      <c r="D32" s="15" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="16"/>
+      <c r="D33" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1823,16 +1835,6 @@
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="R1:X1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:H29;J3:P29;R3:X29">
-    <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(B3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:H29;J3:P29;R3:X29">
-    <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
-      <formula>LEN(TRIM(B3))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>